<commit_message>
Added many test_ functions
</commit_message>
<xml_diff>
--- a/r_package/testing/testing_functions/check PAF.xlsx
+++ b/r_package/testing/testing_functions/check PAF.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12651"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>PAF1</t>
-  </si>
-  <si>
-    <t>PAF2</t>
-  </si>
-  <si>
-    <t>PAF3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Example:</t>
   </si>
@@ -37,6 +28,30 @@
   </si>
   <si>
     <t>prop_pop_exp &lt;- c(0.2, 0.2, 0.6)</t>
+  </si>
+  <si>
+    <t>For exp=8.5</t>
+  </si>
+  <si>
+    <t>PAF lowci</t>
+  </si>
+  <si>
+    <t>PAF3 highci</t>
+  </si>
+  <si>
+    <t>PAF mean</t>
+  </si>
+  <si>
+    <t>Mean rr = 1.118</t>
+  </si>
+  <si>
+    <t>PAF exp = 8.5</t>
+  </si>
+  <si>
+    <t>PAF exp = 13.85</t>
+  </si>
+  <si>
+    <t>PAF exp = 18.85</t>
   </si>
 </sst>
 </file>
@@ -354,58 +369,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.61328125" customWidth="1"/>
+    <col min="2" max="2" width="16.84375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
+      <c r="B5">
         <f>(1.043879-1)*0.2</f>
         <v>8.7758000000000003E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <f>(1.103751-1)*0.2</f>
         <v>2.0750199999999986E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <f>(1.167057-1)*0.6</f>
         <v>0.10023420000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B8">
-        <f>SUM(B4:B6)</f>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B9">
+        <f>SUM(B5:B7)</f>
         <v>0.12976019999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <f>(1.04387884019449-1)*0.2</f>
+        <v>8.775768038898013E-3</v>
+      </c>
+      <c r="D13">
+        <f>(8.85-5)*(1.04387884019449-1)*0.2</f>
+        <v>3.3786706949757349E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <f>(1.10375071048696-1)*0.2</f>
+        <v>2.075014209739199E-2</v>
+      </c>
+      <c r="D14">
+        <f>(13.85-5)*(1.10375071048696-1)*0.2</f>
+        <v>0.18363875756191911</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <f>(1.16705654333744-1)*0.2</f>
+        <v>3.3411308667488003E-2</v>
+      </c>
+      <c r="D15">
+        <f>(18.85-5)*(1.16705654333744-1)*0.6</f>
+        <v>1.3882398751341267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>